<commit_message>
superdataset-21 positive flow only (test with mae)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-4.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-4.xlsx
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,8 +432,12 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="3">
+        <v>84.211330083565429</v>
+      </c>
+      <c r="K5" s="3">
+        <v>236.75963888888879</v>
+      </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
@@ -450,8 +454,12 @@
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="3">
+        <v>84.641448467966583</v>
+      </c>
+      <c r="K6" s="3">
+        <v>218.08497222222221</v>
+      </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
@@ -468,8 +476,12 @@
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="3">
+        <v>84.239004178272964</v>
+      </c>
+      <c r="K7" s="3">
+        <v>215.69088888888879</v>
+      </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
@@ -486,8 +498,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="J8" s="3">
+        <v>83.298426183844001</v>
+      </c>
+      <c r="K8" s="3">
+        <v>231.21124999999989</v>
+      </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
@@ -504,8 +520,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="J9" s="3">
+        <v>81.161559888579404</v>
+      </c>
+      <c r="K9" s="3">
+        <v>243.80224999999999</v>
+      </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
@@ -522,8 +542,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="3">
+        <v>82.456427576601669</v>
+      </c>
+      <c r="K10" s="3">
+        <v>208.3794722222222</v>
+      </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
@@ -540,8 +564,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="J11" s="3">
+        <v>85.929136490250684</v>
+      </c>
+      <c r="K11" s="3">
+        <v>222.09616666666659</v>
+      </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
@@ -558,8 +586,12 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="3">
+        <v>80.713426183844035</v>
+      </c>
+      <c r="K12" s="3">
+        <v>254.3535277777778</v>
+      </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
@@ -576,8 +608,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="J13" s="3">
+        <v>79.992562674094714</v>
+      </c>
+      <c r="K13" s="3">
+        <v>276.0599444444444</v>
+      </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
@@ -594,8 +630,12 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="3">
+        <v>86.018962395543198</v>
+      </c>
+      <c r="K14" s="3">
+        <v>216.13900000000001</v>
+      </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
@@ -612,8 +652,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="J15" s="3">
+        <v>77.790480501392764</v>
+      </c>
+      <c r="K15" s="3">
+        <v>289.13411111111111</v>
+      </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
@@ -630,8 +674,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="J16" s="3">
+        <v>87.079860724233981</v>
+      </c>
+      <c r="K16" s="3">
+        <v>196.1835833333333</v>
+      </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
@@ -648,8 +696,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="J17" s="3">
+        <v>85.728830083565484</v>
+      </c>
+      <c r="K17" s="3">
+        <v>211.1418333333333</v>
+      </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
@@ -666,8 +718,12 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="J18" s="3">
+        <v>83.499707520891349</v>
+      </c>
+      <c r="K18" s="3">
+        <v>207.15077777777771</v>
+      </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
@@ -684,8 +740,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="3">
+        <v>81.553955431754858</v>
+      </c>
+      <c r="K19" s="3">
+        <v>232.8100833333333</v>
+      </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
@@ -702,8 +762,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="J20" s="3">
+        <v>81.184394150417816</v>
+      </c>
+      <c r="K20" s="3">
+        <v>247.53949999999989</v>
+      </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
@@ -720,8 +784,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="J21" s="3">
+        <v>87.361378830083567</v>
+      </c>
+      <c r="K21" s="3">
+        <v>214.29624999999999</v>
+      </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
@@ -738,8 +806,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="J22" s="3">
+        <v>83.945431754874662</v>
+      </c>
+      <c r="K22" s="3">
+        <v>247.0813055555555</v>
+      </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
@@ -756,8 +828,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="J23" s="3">
+        <v>85.912465181058494</v>
+      </c>
+      <c r="K23" s="3">
+        <v>209.3821388888889</v>
+      </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
@@ -774,8 +850,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="J24" s="3">
+        <v>83.985076601671324</v>
+      </c>
+      <c r="K24" s="3">
+        <v>221.24941666666669</v>
+      </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
@@ -792,8 +872,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="J25" s="3">
+        <v>85.065313370473532</v>
+      </c>
+      <c r="K25" s="3">
+        <v>203.49197222222219</v>
+      </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
@@ -810,8 +894,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="J26" s="3">
+        <v>84.341267409470746</v>
+      </c>
+      <c r="K26" s="3">
+        <v>217.5622222222222</v>
+      </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
@@ -828,8 +916,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="J27" s="3">
+        <v>80.737381615598878</v>
+      </c>
+      <c r="K27" s="3">
+        <v>260.94008333333329</v>
+      </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
@@ -846,8 +938,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="J28" s="3">
+        <v>84.611608635097497</v>
+      </c>
+      <c r="K28" s="3">
+        <v>229.2571388888889</v>
+      </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
@@ -864,8 +960,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="J29" s="3">
+        <v>84.272444289693581</v>
+      </c>
+      <c r="K29" s="3">
+        <v>234.03530555555551</v>
+      </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
@@ -882,8 +982,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="J30" s="3">
+        <v>84.459993036211714</v>
+      </c>
+      <c r="K30" s="3">
+        <v>220.39105555555551</v>
+      </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
@@ -900,8 +1004,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="J31" s="3">
+        <v>79.952005571030654</v>
+      </c>
+      <c r="K31" s="3">
+        <v>264.38722222222219</v>
+      </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
@@ -918,8 +1026,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="J32" s="3">
+        <v>81.004213091922011</v>
+      </c>
+      <c r="K32" s="3">
+        <v>218.9157222222222</v>
+      </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
@@ -936,8 +1048,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="J33" s="3">
+        <v>84.973635097493045</v>
+      </c>
+      <c r="K33" s="3">
+        <v>199.01019444444441</v>
+      </c>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
@@ -954,8 +1070,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
+      <c r="J34" s="3">
+        <v>84.822367688022311</v>
+      </c>
+      <c r="K34" s="3">
+        <v>230.27483333333331</v>
+      </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
@@ -972,8 +1092,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
+      <c r="J35" s="3">
+        <v>85.490041782729804</v>
+      </c>
+      <c r="K35" s="3">
+        <v>220.35172222222221</v>
+      </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
@@ -990,8 +1114,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
+      <c r="J36" s="3">
+        <v>81.164679665738163</v>
+      </c>
+      <c r="K36" s="3">
+        <v>244.88677777777781</v>
+      </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
@@ -1008,8 +1136,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
+      <c r="J37" s="3">
+        <v>82.983272980501368</v>
+      </c>
+      <c r="K37" s="3">
+        <v>213.05055555555549</v>
+      </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
@@ -1026,8 +1158,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="J38" s="3">
+        <v>84.37545961002786</v>
+      </c>
+      <c r="K38" s="3">
+        <v>228.0026388888889</v>
+      </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
@@ -1044,8 +1180,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
+      <c r="J39" s="3">
+        <v>81.887576601671313</v>
+      </c>
+      <c r="K39" s="3">
+        <v>251.6039999999999</v>
+      </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
@@ -1062,8 +1202,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="J40" s="3">
+        <v>84.849784122562667</v>
+      </c>
+      <c r="K40" s="3">
+        <v>219.03522222222219</v>
+      </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
@@ -1080,8 +1224,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="J41" s="3">
+        <v>83.412764623955439</v>
+      </c>
+      <c r="K41" s="3">
+        <v>221.97311111111111</v>
+      </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
@@ -1098,8 +1246,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="J42" s="3">
+        <v>85.350090529247908</v>
+      </c>
+      <c r="K42" s="3">
+        <v>199.0651666666667</v>
+      </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
@@ -1116,8 +1268,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
+      <c r="J43" s="3">
+        <v>82.092688022284122</v>
+      </c>
+      <c r="K43" s="3">
+        <v>246.18861111111119</v>
+      </c>
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
@@ -1134,8 +1290,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
+      <c r="J44" s="3">
+        <v>84.253140668523642</v>
+      </c>
+      <c r="K44" s="3">
+        <v>240.04116666666661</v>
+      </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
@@ -1152,8 +1312,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
+      <c r="J45" s="3">
+        <v>85.119136490250725</v>
+      </c>
+      <c r="K45" s="3">
+        <v>228.43741666666659</v>
+      </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
@@ -1170,8 +1334,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
+      <c r="J46" s="3">
+        <v>83.520222841225646</v>
+      </c>
+      <c r="K46" s="3">
+        <v>210.82222222222219</v>
+      </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
@@ -1188,8 +1356,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
+      <c r="J47" s="3">
+        <v>79.662889972144853</v>
+      </c>
+      <c r="K47" s="3">
+        <v>255.65613888888879</v>
+      </c>
     </row>
     <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
@@ -1206,8 +1378,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
+      <c r="J48" s="3">
+        <v>82.973809192200562</v>
+      </c>
+      <c r="K48" s="3">
+        <v>231.96905555555551</v>
+      </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
@@ -1224,8 +1400,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
+      <c r="J49" s="3">
+        <v>84.377367688022289</v>
+      </c>
+      <c r="K49" s="3">
+        <v>231.58827777777779</v>
+      </c>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
@@ -1242,8 +1422,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="J50" s="3">
+        <v>85.085731197771565</v>
+      </c>
+      <c r="K50" s="3">
+        <v>224.00155555555551</v>
+      </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
@@ -1260,8 +1444,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
+      <c r="J51" s="3">
+        <v>82.008850974930368</v>
+      </c>
+      <c r="K51" s="3">
+        <v>270.76558333333332</v>
+      </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
@@ -1278,8 +1466,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="J52" s="3">
+        <v>87.941357938718653</v>
+      </c>
+      <c r="K52" s="3">
+        <v>189.07472222222219</v>
+      </c>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
@@ -1296,8 +1488,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="J53" s="3">
+        <v>84.578934540389966</v>
+      </c>
+      <c r="K53" s="3">
+        <v>236.17058333333341</v>
+      </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
@@ -1314,8 +1510,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+      <c r="J54" s="3">
+        <v>81.476497214484667</v>
+      </c>
+      <c r="K54" s="3">
+        <v>246.71838888888891</v>
+      </c>
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
@@ -1332,13 +1532,13 @@
       <c r="I56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J56" s="3" t="e">
+      <c r="J56" s="3">
         <f>AVERAGE(J5:J54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K56" s="3" t="e">
+        <v>83.550967827298066</v>
+      </c>
+      <c r="K56" s="3">
         <f>AVERAGE(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>229.72429555555547</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
@@ -1356,13 +1556,13 @@
       <c r="I57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="3" t="e">
+      <c r="J57" s="3">
         <f>_xlfn.STDEV.S(J5:J54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K57" s="3" t="e">
+        <v>2.1527115086902144</v>
+      </c>
+      <c r="K57" s="3">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>21.372741716027598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-4 and 6, negative flow corr.
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-4.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -38,12 +38,31 @@
   <si>
     <t>Random Forest-100 (superdataset-21 (positive flow).csv)</t>
   </si>
+  <si>
+    <t>Датасеты с ошибкой (не только год вперед)</t>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Правильные датасеты, прогноз только на год вперед)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +88,21 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -99,6 +133,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -379,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:K57"/>
+  <dimension ref="D2:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,9 +426,21 @@
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
@@ -402,8 +449,16 @@
         <v>5</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -418,8 +473,22 @@
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -438,8 +507,26 @@
       <c r="K5" s="3">
         <v>236.75963888888879</v>
       </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3">
+        <v>31.956522506619589</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>87.735489849955854</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1</v>
+      </c>
+      <c r="U5" s="3">
+        <v>84.211330083565429</v>
+      </c>
+      <c r="V5" s="3">
+        <v>236.75963888888879</v>
+      </c>
+    </row>
+    <row r="6" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -460,8 +547,28 @@
       <c r="K6" s="3">
         <v>218.08497222222221</v>
       </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O6" s="2">
+        <f>O5+1</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="3">
+        <v>32.048040600176513</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>85.456840247131538</v>
+      </c>
+      <c r="T6" s="2">
+        <f>T5+1</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="3">
+        <v>84.641448467966583</v>
+      </c>
+      <c r="V6" s="3">
+        <v>218.08497222222221</v>
+      </c>
+    </row>
+    <row r="7" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -482,8 +589,28 @@
       <c r="K7" s="3">
         <v>215.69088888888879</v>
       </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O7" s="2">
+        <f t="shared" ref="O7:O54" si="2">O6+1</f>
+        <v>3</v>
+      </c>
+      <c r="P7" s="3">
+        <v>31.827705207413931</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>83.746478375992936</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" ref="T7:T54" si="3">T6+1</f>
+        <v>3</v>
+      </c>
+      <c r="U7" s="3">
+        <v>84.239004178272964</v>
+      </c>
+      <c r="V7" s="3">
+        <v>215.69088888888879</v>
+      </c>
+    </row>
+    <row r="8" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -504,8 +631,28 @@
       <c r="K8" s="3">
         <v>231.21124999999989</v>
       </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>32.607976610767871</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>85.950609002647852</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U8" s="3">
+        <v>83.298426183844001</v>
+      </c>
+      <c r="V8" s="3">
+        <v>231.21124999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -526,8 +673,28 @@
       <c r="K9" s="3">
         <v>243.80224999999999</v>
       </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P9" s="3">
+        <v>32.358102383053833</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>89.994510150044135</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U9" s="3">
+        <v>81.161559888579404</v>
+      </c>
+      <c r="V9" s="3">
+        <v>243.80224999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -548,8 +715,28 @@
       <c r="K10" s="3">
         <v>208.3794722222222</v>
       </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P10" s="3">
+        <v>31.885059576345981</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>85.550070609002645</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="U10" s="3">
+        <v>82.456427576601669</v>
+      </c>
+      <c r="V10" s="3">
+        <v>208.3794722222222</v>
+      </c>
+    </row>
+    <row r="11" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -570,8 +757,28 @@
       <c r="K11" s="3">
         <v>222.09616666666659</v>
       </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="P11" s="3">
+        <v>32.026950573698137</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>86.81519858781995</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U11" s="3">
+        <v>85.929136490250684</v>
+      </c>
+      <c r="V11" s="3">
+        <v>222.09616666666659</v>
+      </c>
+    </row>
+    <row r="12" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -592,8 +799,28 @@
       <c r="K12" s="3">
         <v>254.3535277777778</v>
       </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="P12" s="3">
+        <v>31.929143865842889</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>85.153971756398931</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U12" s="3">
+        <v>80.713426183844035</v>
+      </c>
+      <c r="V12" s="3">
+        <v>254.3535277777778</v>
+      </c>
+    </row>
+    <row r="13" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -614,8 +841,28 @@
       <c r="K13" s="3">
         <v>276.0599444444444</v>
       </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="P13" s="3">
+        <v>32.370039717563976</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>87.09514563106795</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="U13" s="3">
+        <v>79.992562674094714</v>
+      </c>
+      <c r="V13" s="3">
+        <v>276.0599444444444</v>
+      </c>
+    </row>
+    <row r="14" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -636,8 +883,28 @@
       <c r="K14" s="3">
         <v>216.13900000000001</v>
       </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="P14" s="3">
+        <v>31.90246690203</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>87.007705207413949</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="U14" s="3">
+        <v>86.018962395543198</v>
+      </c>
+      <c r="V14" s="3">
+        <v>216.13900000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -658,8 +925,28 @@
       <c r="K15" s="3">
         <v>289.13411111111111</v>
       </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P15" s="3">
+        <v>31.945887025595759</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>87.413150926743171</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="U15" s="3">
+        <v>77.790480501392764</v>
+      </c>
+      <c r="V15" s="3">
+        <v>289.13411111111111</v>
+      </c>
+    </row>
+    <row r="16" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -680,8 +967,28 @@
       <c r="K16" s="3">
         <v>196.1835833333333</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P16" s="3">
+        <v>31.892493380405998</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>88.328905560458963</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="U16" s="3">
+        <v>87.079860724233981</v>
+      </c>
+      <c r="V16" s="3">
+        <v>196.1835833333333</v>
+      </c>
+    </row>
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -702,8 +1009,28 @@
       <c r="K17" s="3">
         <v>211.1418333333333</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P17" s="3">
+        <v>32.58850617828773</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>81.741676963812893</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="U17" s="3">
+        <v>85.728830083565484</v>
+      </c>
+      <c r="V17" s="3">
+        <v>211.1418333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -724,8 +1051,28 @@
       <c r="K18" s="3">
         <v>207.15077777777771</v>
       </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P18" s="3">
+        <v>32.13540158870255</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>86.175207413945287</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="U18" s="3">
+        <v>83.499707520891349</v>
+      </c>
+      <c r="V18" s="3">
+        <v>207.15077777777771</v>
+      </c>
+    </row>
+    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -746,8 +1093,28 @@
       <c r="K19" s="3">
         <v>232.8100833333333</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P19" s="3">
+        <v>31.95389894086496</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>87.055225066195945</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="U19" s="3">
+        <v>81.553955431754858</v>
+      </c>
+      <c r="V19" s="3">
+        <v>232.8100833333333</v>
+      </c>
+    </row>
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -768,8 +1135,28 @@
       <c r="K20" s="3">
         <v>247.53949999999989</v>
       </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="P20" s="3">
+        <v>32.204905119152691</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>83.02304501323917</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="U20" s="3">
+        <v>81.184394150417816</v>
+      </c>
+      <c r="V20" s="3">
+        <v>247.53949999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -790,8 +1177,28 @@
       <c r="K21" s="3">
         <v>214.29624999999999</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="P21" s="3">
+        <v>31.9515026478376</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>87.459708737864077</v>
+      </c>
+      <c r="T21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="U21" s="3">
+        <v>87.361378830083567</v>
+      </c>
+      <c r="V21" s="3">
+        <v>214.29624999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -812,8 +1219,28 @@
       <c r="K22" s="3">
         <v>247.0813055555555</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="P22" s="3">
+        <v>31.901418799646951</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>89.990370697263913</v>
+      </c>
+      <c r="T22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="U22" s="3">
+        <v>83.945431754874662</v>
+      </c>
+      <c r="V22" s="3">
+        <v>247.0813055555555</v>
+      </c>
+    </row>
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -834,8 +1261,28 @@
       <c r="K23" s="3">
         <v>209.3821388888889</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="P23" s="3">
+        <v>31.981387908208291</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>89.483459841129743</v>
+      </c>
+      <c r="T23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="U23" s="3">
+        <v>85.912465181058494</v>
+      </c>
+      <c r="V23" s="3">
+        <v>209.3821388888889</v>
+      </c>
+    </row>
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -856,8 +1303,28 @@
       <c r="K24" s="3">
         <v>221.24941666666669</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P24" s="3">
+        <v>31.939274051191521</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>90.01291262135922</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="U24" s="3">
+        <v>83.985076601671324</v>
+      </c>
+      <c r="V24" s="3">
+        <v>221.24941666666669</v>
+      </c>
+    </row>
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -878,8 +1345,28 @@
       <c r="K25" s="3">
         <v>203.49197222222219</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="P25" s="3">
+        <v>31.98178508384818</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>86.684077669902905</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="U25" s="3">
+        <v>85.065313370473532</v>
+      </c>
+      <c r="V25" s="3">
+        <v>203.49197222222219</v>
+      </c>
+    </row>
+    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -900,8 +1387,28 @@
       <c r="K26" s="3">
         <v>217.5622222222222</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="P26" s="3">
+        <v>32.387513239187989</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>83.304554280670786</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="U26" s="3">
+        <v>84.341267409470746</v>
+      </c>
+      <c r="V26" s="3">
+        <v>217.5622222222222</v>
+      </c>
+    </row>
+    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -922,8 +1429,28 @@
       <c r="K27" s="3">
         <v>260.94008333333329</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="P27" s="3">
+        <v>31.892080759046781</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>88.188172992056494</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="U27" s="3">
+        <v>80.737381615598878</v>
+      </c>
+      <c r="V27" s="3">
+        <v>260.94008333333329</v>
+      </c>
+    </row>
+    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -944,8 +1471,28 @@
       <c r="K28" s="3">
         <v>229.2571388888889</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="P28" s="3">
+        <v>31.98385701676964</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>86.713009708737872</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="U28" s="3">
+        <v>84.611608635097497</v>
+      </c>
+      <c r="V28" s="3">
+        <v>229.2571388888889</v>
+      </c>
+    </row>
+    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -966,8 +1513,28 @@
       <c r="K29" s="3">
         <v>234.03530555555551</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="P29" s="3">
+        <v>31.879304942630181</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>90.182656663724629</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="U29" s="3">
+        <v>84.272444289693581</v>
+      </c>
+      <c r="V29" s="3">
+        <v>234.03530555555551</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -988,8 +1555,28 @@
       <c r="K30" s="3">
         <v>220.39105555555551</v>
       </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="P30" s="3">
+        <v>32.052365401588702</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>88.405586937334519</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="U30" s="3">
+        <v>84.459993036211714</v>
+      </c>
+      <c r="V30" s="3">
+        <v>220.39105555555551</v>
+      </c>
+    </row>
+    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1010,8 +1597,28 @@
       <c r="K31" s="3">
         <v>264.38722222222219</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P31" s="3">
+        <v>32.077153574580763</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>84.239232127096201</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="U31" s="3">
+        <v>79.952005571030654</v>
+      </c>
+      <c r="V31" s="3">
+        <v>264.38722222222219</v>
+      </c>
+    </row>
+    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1032,8 +1639,28 @@
       <c r="K32" s="3">
         <v>218.9157222222222</v>
       </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="P32" s="3">
+        <v>32.374880847308027</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>82.617290379523396</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="U32" s="3">
+        <v>81.004213091922011</v>
+      </c>
+      <c r="V32" s="3">
+        <v>218.9157222222222</v>
+      </c>
+    </row>
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1054,8 +1681,28 @@
       <c r="K33" s="3">
         <v>199.01019444444441</v>
       </c>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="P33" s="3">
+        <v>31.74499117387467</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>88.046831421006189</v>
+      </c>
+      <c r="T33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="U33" s="3">
+        <v>84.973635097493045</v>
+      </c>
+      <c r="V33" s="3">
+        <v>199.01019444444441</v>
+      </c>
+    </row>
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1076,8 +1723,28 @@
       <c r="K34" s="3">
         <v>230.27483333333331</v>
       </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="P34" s="3">
+        <v>32.283762135922323</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>84.775180935569296</v>
+      </c>
+      <c r="T34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="U34" s="3">
+        <v>84.822367688022311</v>
+      </c>
+      <c r="V34" s="3">
+        <v>230.27483333333331</v>
+      </c>
+    </row>
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1098,8 +1765,28 @@
       <c r="K35" s="3">
         <v>220.35172222222221</v>
       </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="P35" s="3">
+        <v>31.8616107678729</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>87.887087378640786</v>
+      </c>
+      <c r="T35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="U35" s="3">
+        <v>85.490041782729804</v>
+      </c>
+      <c r="V35" s="3">
+        <v>220.35172222222221</v>
+      </c>
+    </row>
+    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1120,8 +1807,28 @@
       <c r="K36" s="3">
         <v>244.88677777777781</v>
       </c>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="P36" s="3">
+        <v>32.219940423654023</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>86.819408649602806</v>
+      </c>
+      <c r="T36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="U36" s="3">
+        <v>81.164679665738163</v>
+      </c>
+      <c r="V36" s="3">
+        <v>244.88677777777781</v>
+      </c>
+    </row>
+    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1142,8 +1849,28 @@
       <c r="K37" s="3">
         <v>213.05055555555549</v>
       </c>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="P37" s="3">
+        <v>32.289243159752857</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>83.072524271844671</v>
+      </c>
+      <c r="T37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="U37" s="3">
+        <v>82.983272980501368</v>
+      </c>
+      <c r="V37" s="3">
+        <v>213.05055555555549</v>
+      </c>
+    </row>
+    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1164,8 +1891,28 @@
       <c r="K38" s="3">
         <v>228.0026388888889</v>
       </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="P38" s="3">
+        <v>32.222480141217993</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>87.114624889673436</v>
+      </c>
+      <c r="T38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="U38" s="3">
+        <v>84.37545961002786</v>
+      </c>
+      <c r="V38" s="3">
+        <v>228.0026388888889</v>
+      </c>
+    </row>
+    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1186,8 +1933,28 @@
       <c r="K39" s="3">
         <v>251.6039999999999</v>
       </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="P39" s="3">
+        <v>32.004702118270068</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>84.430247131509262</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="U39" s="3">
+        <v>81.887576601671313</v>
+      </c>
+      <c r="V39" s="3">
+        <v>251.6039999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1208,8 +1975,28 @@
       <c r="K40" s="3">
         <v>219.03522222222219</v>
       </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="P40" s="3">
+        <v>31.7631200353045</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>91.781535745807574</v>
+      </c>
+      <c r="T40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="U40" s="3">
+        <v>84.849784122562667</v>
+      </c>
+      <c r="V40" s="3">
+        <v>219.03522222222219</v>
+      </c>
+    </row>
+    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1230,8 +2017,28 @@
       <c r="K41" s="3">
         <v>221.97311111111111</v>
       </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="P41" s="3">
+        <v>32.418161959399818</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>83.659832303618728</v>
+      </c>
+      <c r="T41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="U41" s="3">
+        <v>83.412764623955439</v>
+      </c>
+      <c r="V41" s="3">
+        <v>221.97311111111111</v>
+      </c>
+    </row>
+    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1252,8 +2059,28 @@
       <c r="K42" s="3">
         <v>199.0651666666667</v>
       </c>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="P42" s="3">
+        <v>31.87679170344218</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>88.156390114739636</v>
+      </c>
+      <c r="T42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="U42" s="3">
+        <v>85.350090529247908</v>
+      </c>
+      <c r="V42" s="3">
+        <v>199.0651666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1274,8 +2101,28 @@
       <c r="K43" s="3">
         <v>246.18861111111119</v>
       </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="P43" s="3">
+        <v>31.512546337157989</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>88.272877316857901</v>
+      </c>
+      <c r="T43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="U43" s="3">
+        <v>82.092688022284122</v>
+      </c>
+      <c r="V43" s="3">
+        <v>246.18861111111119</v>
+      </c>
+    </row>
+    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1296,8 +2143,28 @@
       <c r="K44" s="3">
         <v>240.04116666666661</v>
       </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="P44" s="3">
+        <v>32.101994704324802</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>85.886028243601075</v>
+      </c>
+      <c r="T44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="U44" s="3">
+        <v>84.253140668523642</v>
+      </c>
+      <c r="V44" s="3">
+        <v>240.04116666666661</v>
+      </c>
+    </row>
+    <row r="45" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1318,8 +2185,28 @@
       <c r="K45" s="3">
         <v>228.43741666666659</v>
       </c>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="P45" s="3">
+        <v>32.021451897616942</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>84.81916151809358</v>
+      </c>
+      <c r="T45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="U45" s="3">
+        <v>85.119136490250725</v>
+      </c>
+      <c r="V45" s="3">
+        <v>228.43741666666659</v>
+      </c>
+    </row>
+    <row r="46" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1340,8 +2227,28 @@
       <c r="K46" s="3">
         <v>210.82222222222219</v>
       </c>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="P46" s="3">
+        <v>31.33616946160635</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>92.832065313327448</v>
+      </c>
+      <c r="T46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="U46" s="3">
+        <v>83.520222841225646</v>
+      </c>
+      <c r="V46" s="3">
+        <v>210.82222222222219</v>
+      </c>
+    </row>
+    <row r="47" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1362,8 +2269,28 @@
       <c r="K47" s="3">
         <v>255.65613888888879</v>
       </c>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="P47" s="3">
+        <v>32.24772506619594</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>86.4573168578994</v>
+      </c>
+      <c r="T47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="U47" s="3">
+        <v>79.662889972144853</v>
+      </c>
+      <c r="V47" s="3">
+        <v>255.65613888888879</v>
+      </c>
+    </row>
+    <row r="48" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1384,8 +2311,28 @@
       <c r="K48" s="3">
         <v>231.96905555555551</v>
       </c>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="P48" s="3">
+        <v>31.843349514563101</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>92.630008826125348</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="U48" s="3">
+        <v>82.973809192200562</v>
+      </c>
+      <c r="V48" s="3">
+        <v>231.96905555555551</v>
+      </c>
+    </row>
+    <row r="49" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1406,8 +2353,28 @@
       <c r="K49" s="3">
         <v>231.58827777777779</v>
       </c>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="P49" s="3">
+        <v>32.075904677846417</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>87.392630185348636</v>
+      </c>
+      <c r="T49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="U49" s="3">
+        <v>84.377367688022289</v>
+      </c>
+      <c r="V49" s="3">
+        <v>231.58827777777779</v>
+      </c>
+    </row>
+    <row r="50" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1428,8 +2395,28 @@
       <c r="K50" s="3">
         <v>224.00155555555551</v>
       </c>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="P50" s="3">
+        <v>32.138598852603707</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>87.319232127096228</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="U50" s="3">
+        <v>85.085731197771565</v>
+      </c>
+      <c r="V50" s="3">
+        <v>224.00155555555551</v>
+      </c>
+    </row>
+    <row r="51" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1450,8 +2437,28 @@
       <c r="K51" s="3">
         <v>270.76558333333332</v>
       </c>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="P51" s="3">
+        <v>32.212440423654023</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>88.674139452780253</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="U51" s="3">
+        <v>82.008850974930368</v>
+      </c>
+      <c r="V51" s="3">
+        <v>270.76558333333332</v>
+      </c>
+    </row>
+    <row r="52" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1472,8 +2479,28 @@
       <c r="K52" s="3">
         <v>189.07472222222219</v>
       </c>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="P52" s="3">
+        <v>31.847330097087369</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>87.30729037952338</v>
+      </c>
+      <c r="T52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="U52" s="3">
+        <v>87.941357938718653</v>
+      </c>
+      <c r="V52" s="3">
+        <v>189.07472222222219</v>
+      </c>
+    </row>
+    <row r="53" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1494,8 +2521,28 @@
       <c r="K53" s="3">
         <v>236.17058333333341</v>
       </c>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="P53" s="3">
+        <v>31.770867166813769</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>89.480582524271853</v>
+      </c>
+      <c r="T53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="U53" s="3">
+        <v>84.578934540389966</v>
+      </c>
+      <c r="V53" s="3">
+        <v>236.17058333333341</v>
+      </c>
+    </row>
+    <row r="54" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1516,8 +2563,28 @@
       <c r="K54" s="3">
         <v>246.71838888888891</v>
       </c>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="P54" s="3">
+        <v>31.57947263901147</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>90.014872021182697</v>
+      </c>
+      <c r="T54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="U54" s="3">
+        <v>81.476497214484667</v>
+      </c>
+      <c r="V54" s="3">
+        <v>246.71838888888891</v>
+      </c>
+    </row>
+    <row r="56" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1540,8 +2607,30 @@
         <f>AVERAGE(K5:K54)</f>
         <v>229.72429555555547</v>
       </c>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P56" s="3">
+        <f>AVERAGE(P5:P54)</f>
+        <v>32.028165578111228</v>
+      </c>
+      <c r="Q56" s="3">
+        <f>AVERAGE(Q5:Q54)</f>
+        <v>87.047082612533103</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U56" s="3">
+        <f>AVERAGE(U5:U54)</f>
+        <v>83.550967827298066</v>
+      </c>
+      <c r="V56" s="3">
+        <f>AVERAGE(V5:V54)</f>
+        <v>229.72429555555547</v>
+      </c>
+    </row>
+    <row r="57" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1564,8 +2653,31 @@
         <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>21.372741716027598</v>
       </c>
+      <c r="O57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P57" s="3">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>0.25206438068763098</v>
+      </c>
+      <c r="Q57" s="3">
+        <f>_xlfn.STDEV.S(Q5:Q54)</f>
+        <v>2.5151399869449298</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U57" s="3">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
+        <v>2.1527115086902144</v>
+      </c>
+      <c r="V57" s="3">
+        <f>_xlfn.STDEV.S(V5:V54)</f>
+        <v>21.372741716027598</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test-4 and 6, positive flow corr.
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-4.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-4.xlsx
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="U5" s="3">
-        <v>84.211330083565429</v>
+        <v>92.642549371633763</v>
       </c>
       <c r="V5" s="3">
-        <v>236.75963888888879</v>
+        <v>274.09863799283153</v>
       </c>
     </row>
     <row r="6" spans="4:22" x14ac:dyDescent="0.25">
@@ -562,10 +562,10 @@
         <v>2</v>
       </c>
       <c r="U6" s="3">
-        <v>84.641448467966583</v>
+        <v>89.769021543985616</v>
       </c>
       <c r="V6" s="3">
-        <v>218.08497222222221</v>
+        <v>271.86967741935479</v>
       </c>
     </row>
     <row r="7" spans="4:22" x14ac:dyDescent="0.25">
@@ -604,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="U7" s="3">
-        <v>84.239004178272964</v>
+        <v>93.825897666068215</v>
       </c>
       <c r="V7" s="3">
-        <v>215.69088888888879</v>
+        <v>257.52014336917563</v>
       </c>
     </row>
     <row r="8" spans="4:22" x14ac:dyDescent="0.25">
@@ -646,10 +646,10 @@
         <v>4</v>
       </c>
       <c r="U8" s="3">
-        <v>83.298426183844001</v>
+        <v>94.217118491920999</v>
       </c>
       <c r="V8" s="3">
-        <v>231.21124999999989</v>
+        <v>219.121505376344</v>
       </c>
     </row>
     <row r="9" spans="4:22" x14ac:dyDescent="0.25">
@@ -688,10 +688,10 @@
         <v>5</v>
       </c>
       <c r="U9" s="3">
-        <v>81.161559888579404</v>
+        <v>93.87625673249552</v>
       </c>
       <c r="V9" s="3">
-        <v>243.80224999999999</v>
+        <v>234.62623655913981</v>
       </c>
     </row>
     <row r="10" spans="4:22" x14ac:dyDescent="0.25">
@@ -730,10 +730,10 @@
         <v>6</v>
       </c>
       <c r="U10" s="3">
-        <v>82.456427576601669</v>
+        <v>96.123078994613991</v>
       </c>
       <c r="V10" s="3">
-        <v>208.3794722222222</v>
+        <v>226.21516129032261</v>
       </c>
     </row>
     <row r="11" spans="4:22" x14ac:dyDescent="0.25">
@@ -772,10 +772,10 @@
         <v>7</v>
       </c>
       <c r="U11" s="3">
-        <v>85.929136490250684</v>
+        <v>93.578698384201076</v>
       </c>
       <c r="V11" s="3">
-        <v>222.09616666666659</v>
+        <v>236.87544802867379</v>
       </c>
     </row>
     <row r="12" spans="4:22" x14ac:dyDescent="0.25">
@@ -814,10 +814,10 @@
         <v>8</v>
       </c>
       <c r="U12" s="3">
-        <v>80.713426183844035</v>
+        <v>96.080520646319556</v>
       </c>
       <c r="V12" s="3">
-        <v>254.3535277777778</v>
+        <v>207.84261648745519</v>
       </c>
     </row>
     <row r="13" spans="4:22" x14ac:dyDescent="0.25">
@@ -856,10 +856,10 @@
         <v>9</v>
       </c>
       <c r="U13" s="3">
-        <v>79.992562674094714</v>
+        <v>92.845224416517041</v>
       </c>
       <c r="V13" s="3">
-        <v>276.0599444444444</v>
+        <v>268.41956989247308</v>
       </c>
     </row>
     <row r="14" spans="4:22" x14ac:dyDescent="0.25">
@@ -898,10 +898,10 @@
         <v>10</v>
       </c>
       <c r="U14" s="3">
-        <v>86.018962395543198</v>
+        <v>89.017764811490139</v>
       </c>
       <c r="V14" s="3">
-        <v>216.13900000000001</v>
+        <v>282.54508960573469</v>
       </c>
     </row>
     <row r="15" spans="4:22" x14ac:dyDescent="0.25">
@@ -940,10 +940,10 @@
         <v>11</v>
       </c>
       <c r="U15" s="3">
-        <v>77.790480501392764</v>
+        <v>91.695197486535008</v>
       </c>
       <c r="V15" s="3">
-        <v>289.13411111111111</v>
+        <v>249.3034767025089</v>
       </c>
     </row>
     <row r="16" spans="4:22" x14ac:dyDescent="0.25">
@@ -982,10 +982,10 @@
         <v>12</v>
       </c>
       <c r="U16" s="3">
-        <v>87.079860724233981</v>
+        <v>97.161113105924585</v>
       </c>
       <c r="V16" s="3">
-        <v>196.1835833333333</v>
+        <v>238.25903225806451</v>
       </c>
     </row>
     <row r="17" spans="4:22" x14ac:dyDescent="0.25">
@@ -1024,10 +1024,10 @@
         <v>13</v>
       </c>
       <c r="U17" s="3">
-        <v>85.728830083565484</v>
+        <v>94.144470377019744</v>
       </c>
       <c r="V17" s="3">
-        <v>211.1418333333333</v>
+        <v>250.61698924731189</v>
       </c>
     </row>
     <row r="18" spans="4:22" x14ac:dyDescent="0.25">
@@ -1066,10 +1066,10 @@
         <v>14</v>
       </c>
       <c r="U18" s="3">
-        <v>83.499707520891349</v>
+        <v>92.937692998204653</v>
       </c>
       <c r="V18" s="3">
-        <v>207.15077777777771</v>
+        <v>220.14394265232971</v>
       </c>
     </row>
     <row r="19" spans="4:22" x14ac:dyDescent="0.25">
@@ -1108,10 +1108,10 @@
         <v>15</v>
       </c>
       <c r="U19" s="3">
-        <v>81.553955431754858</v>
+        <v>93.197989228007188</v>
       </c>
       <c r="V19" s="3">
-        <v>232.8100833333333</v>
+        <v>248.44781362007171</v>
       </c>
     </row>
     <row r="20" spans="4:22" x14ac:dyDescent="0.25">
@@ -1150,10 +1150,10 @@
         <v>16</v>
       </c>
       <c r="U20" s="3">
-        <v>81.184394150417816</v>
+        <v>92.752136445242328</v>
       </c>
       <c r="V20" s="3">
-        <v>247.53949999999989</v>
+        <v>268.69372759856628</v>
       </c>
     </row>
     <row r="21" spans="4:22" x14ac:dyDescent="0.25">
@@ -1192,10 +1192,10 @@
         <v>17</v>
       </c>
       <c r="U21" s="3">
-        <v>87.361378830083567</v>
+        <v>94.798195691202906</v>
       </c>
       <c r="V21" s="3">
-        <v>214.29624999999999</v>
+        <v>246.5005017921147</v>
       </c>
     </row>
     <row r="22" spans="4:22" x14ac:dyDescent="0.25">
@@ -1234,10 +1234,10 @@
         <v>18</v>
       </c>
       <c r="U22" s="3">
-        <v>83.945431754874662</v>
+        <v>97.218644524236979</v>
       </c>
       <c r="V22" s="3">
-        <v>247.0813055555555</v>
+        <v>213.99060931899649</v>
       </c>
     </row>
     <row r="23" spans="4:22" x14ac:dyDescent="0.25">
@@ -1276,10 +1276,10 @@
         <v>19</v>
       </c>
       <c r="U23" s="3">
-        <v>85.912465181058494</v>
+        <v>90.219353680430885</v>
       </c>
       <c r="V23" s="3">
-        <v>209.3821388888889</v>
+        <v>263.60681003584227</v>
       </c>
     </row>
     <row r="24" spans="4:22" x14ac:dyDescent="0.25">
@@ -1318,10 +1318,10 @@
         <v>20</v>
       </c>
       <c r="U24" s="3">
-        <v>83.985076601671324</v>
+        <v>94.489488330341104</v>
       </c>
       <c r="V24" s="3">
-        <v>221.24941666666669</v>
+        <v>227.25892473118279</v>
       </c>
     </row>
     <row r="25" spans="4:22" x14ac:dyDescent="0.25">
@@ -1360,10 +1360,10 @@
         <v>21</v>
       </c>
       <c r="U25" s="3">
-        <v>85.065313370473532</v>
+        <v>95.683276481149008</v>
       </c>
       <c r="V25" s="3">
-        <v>203.49197222222219</v>
+        <v>210.81878136200709</v>
       </c>
     </row>
     <row r="26" spans="4:22" x14ac:dyDescent="0.25">
@@ -1402,10 +1402,10 @@
         <v>22</v>
       </c>
       <c r="U26" s="3">
-        <v>84.341267409470746</v>
+        <v>93.392387791741442</v>
       </c>
       <c r="V26" s="3">
-        <v>217.5622222222222</v>
+        <v>249.69641577060929</v>
       </c>
     </row>
     <row r="27" spans="4:22" x14ac:dyDescent="0.25">
@@ -1444,10 +1444,10 @@
         <v>23</v>
       </c>
       <c r="U27" s="3">
-        <v>80.737381615598878</v>
+        <v>96.263608617594244</v>
       </c>
       <c r="V27" s="3">
-        <v>260.94008333333329</v>
+        <v>225.14530465949821</v>
       </c>
     </row>
     <row r="28" spans="4:22" x14ac:dyDescent="0.25">
@@ -1486,10 +1486,10 @@
         <v>24</v>
       </c>
       <c r="U28" s="3">
-        <v>84.611608635097497</v>
+        <v>93.765502692998183</v>
       </c>
       <c r="V28" s="3">
-        <v>229.2571388888889</v>
+        <v>243.99630824372761</v>
       </c>
     </row>
     <row r="29" spans="4:22" x14ac:dyDescent="0.25">
@@ -1528,10 +1528,10 @@
         <v>25</v>
       </c>
       <c r="U29" s="3">
-        <v>84.272444289693581</v>
+        <v>91.28363554757631</v>
       </c>
       <c r="V29" s="3">
-        <v>234.03530555555551</v>
+        <v>277.64168458781359</v>
       </c>
     </row>
     <row r="30" spans="4:22" x14ac:dyDescent="0.25">
@@ -1570,10 +1570,10 @@
         <v>26</v>
       </c>
       <c r="U30" s="3">
-        <v>84.459993036211714</v>
+        <v>88.575314183123893</v>
       </c>
       <c r="V30" s="3">
-        <v>220.39105555555551</v>
+        <v>279.51362007168461</v>
       </c>
     </row>
     <row r="31" spans="4:22" x14ac:dyDescent="0.25">
@@ -1612,10 +1612,10 @@
         <v>27</v>
       </c>
       <c r="U31" s="3">
-        <v>79.952005571030654</v>
+        <v>94.984021543985605</v>
       </c>
       <c r="V31" s="3">
-        <v>264.38722222222219</v>
+        <v>217.1860215053764</v>
       </c>
     </row>
     <row r="32" spans="4:22" x14ac:dyDescent="0.25">
@@ -1654,10 +1654,10 @@
         <v>28</v>
       </c>
       <c r="U32" s="3">
-        <v>81.004213091922011</v>
+        <v>83.28699281867145</v>
       </c>
       <c r="V32" s="3">
-        <v>218.9157222222222</v>
+        <v>306.21673835125449</v>
       </c>
     </row>
     <row r="33" spans="4:22" x14ac:dyDescent="0.25">
@@ -1696,10 +1696,10 @@
         <v>29</v>
       </c>
       <c r="U33" s="3">
-        <v>84.973635097493045</v>
+        <v>89.033267504488322</v>
       </c>
       <c r="V33" s="3">
-        <v>199.01019444444441</v>
+        <v>273.25093189964161</v>
       </c>
     </row>
     <row r="34" spans="4:22" x14ac:dyDescent="0.25">
@@ -1738,10 +1738,10 @@
         <v>30</v>
       </c>
       <c r="U34" s="3">
-        <v>84.822367688022311</v>
+        <v>92.136256732495511</v>
       </c>
       <c r="V34" s="3">
-        <v>230.27483333333331</v>
+        <v>260.85071684587808</v>
       </c>
     </row>
     <row r="35" spans="4:22" x14ac:dyDescent="0.25">
@@ -1780,10 +1780,10 @@
         <v>31</v>
       </c>
       <c r="U35" s="3">
-        <v>85.490041782729804</v>
+        <v>87.797746858168736</v>
       </c>
       <c r="V35" s="3">
-        <v>220.35172222222221</v>
+        <v>287.94093189964161</v>
       </c>
     </row>
     <row r="36" spans="4:22" x14ac:dyDescent="0.25">
@@ -1822,10 +1822,10 @@
         <v>32</v>
       </c>
       <c r="U36" s="3">
-        <v>81.164679665738163</v>
+        <v>93.917307001795308</v>
       </c>
       <c r="V36" s="3">
-        <v>244.88677777777781</v>
+        <v>242.27462365591401</v>
       </c>
     </row>
     <row r="37" spans="4:22" x14ac:dyDescent="0.25">
@@ -1864,10 +1864,10 @@
         <v>33</v>
       </c>
       <c r="U37" s="3">
-        <v>82.983272980501368</v>
+        <v>93.437728904847404</v>
       </c>
       <c r="V37" s="3">
-        <v>213.05055555555549</v>
+        <v>245.58989247311831</v>
       </c>
     </row>
     <row r="38" spans="4:22" x14ac:dyDescent="0.25">
@@ -1906,10 +1906,10 @@
         <v>34</v>
       </c>
       <c r="U38" s="3">
-        <v>84.37545961002786</v>
+        <v>92.17074506283663</v>
       </c>
       <c r="V38" s="3">
-        <v>228.0026388888889</v>
+        <v>268.59326164874551</v>
       </c>
     </row>
     <row r="39" spans="4:22" x14ac:dyDescent="0.25">
@@ -1948,10 +1948,10 @@
         <v>35</v>
       </c>
       <c r="U39" s="3">
-        <v>81.887576601671313</v>
+        <v>89.983456014362645</v>
       </c>
       <c r="V39" s="3">
-        <v>251.6039999999999</v>
+        <v>272.0548028673835</v>
       </c>
     </row>
     <row r="40" spans="4:22" x14ac:dyDescent="0.25">
@@ -1990,10 +1990,10 @@
         <v>36</v>
       </c>
       <c r="U40" s="3">
-        <v>84.849784122562667</v>
+        <v>94.569425493716309</v>
       </c>
       <c r="V40" s="3">
-        <v>219.03522222222219</v>
+        <v>248.78236559139779</v>
       </c>
     </row>
     <row r="41" spans="4:22" x14ac:dyDescent="0.25">
@@ -2032,10 +2032,10 @@
         <v>37</v>
       </c>
       <c r="U41" s="3">
-        <v>83.412764623955439</v>
+        <v>91.909066427289048</v>
       </c>
       <c r="V41" s="3">
-        <v>221.97311111111111</v>
+        <v>237.23240143369171</v>
       </c>
     </row>
     <row r="42" spans="4:22" x14ac:dyDescent="0.25">
@@ -2074,10 +2074,10 @@
         <v>38</v>
       </c>
       <c r="U42" s="3">
-        <v>85.350090529247908</v>
+        <v>94.01766606822261</v>
       </c>
       <c r="V42" s="3">
-        <v>199.0651666666667</v>
+        <v>254.03189964157701</v>
       </c>
     </row>
     <row r="43" spans="4:22" x14ac:dyDescent="0.25">
@@ -2116,10 +2116,10 @@
         <v>39</v>
       </c>
       <c r="U43" s="3">
-        <v>82.092688022284122</v>
+        <v>93.028357271095146</v>
       </c>
       <c r="V43" s="3">
-        <v>246.18861111111119</v>
+        <v>233.10315412186381</v>
       </c>
     </row>
     <row r="44" spans="4:22" x14ac:dyDescent="0.25">
@@ -2158,10 +2158,10 @@
         <v>40</v>
       </c>
       <c r="U44" s="3">
-        <v>84.253140668523642</v>
+        <v>91.381508078994614</v>
       </c>
       <c r="V44" s="3">
-        <v>240.04116666666661</v>
+        <v>256.04569892473131</v>
       </c>
     </row>
     <row r="45" spans="4:22" x14ac:dyDescent="0.25">
@@ -2200,10 +2200,10 @@
         <v>41</v>
       </c>
       <c r="U45" s="3">
-        <v>85.119136490250725</v>
+        <v>94.49012567324958</v>
       </c>
       <c r="V45" s="3">
-        <v>228.43741666666659</v>
+        <v>243.04304659498209</v>
       </c>
     </row>
     <row r="46" spans="4:22" x14ac:dyDescent="0.25">
@@ -2242,10 +2242,10 @@
         <v>42</v>
       </c>
       <c r="U46" s="3">
-        <v>83.520222841225646</v>
+        <v>94.661777378815074</v>
       </c>
       <c r="V46" s="3">
-        <v>210.82222222222219</v>
+        <v>241.33985663082441</v>
       </c>
     </row>
     <row r="47" spans="4:22" x14ac:dyDescent="0.25">
@@ -2284,10 +2284,10 @@
         <v>43</v>
       </c>
       <c r="U47" s="3">
-        <v>79.662889972144853</v>
+        <v>91.879479353680409</v>
       </c>
       <c r="V47" s="3">
-        <v>255.65613888888879</v>
+        <v>260.28910394265228</v>
       </c>
     </row>
     <row r="48" spans="4:22" x14ac:dyDescent="0.25">
@@ -2326,10 +2326,10 @@
         <v>44</v>
       </c>
       <c r="U48" s="3">
-        <v>82.973809192200562</v>
+        <v>94.769272890484743</v>
       </c>
       <c r="V48" s="3">
-        <v>231.96905555555551</v>
+        <v>218.34211469534051</v>
       </c>
     </row>
     <row r="49" spans="4:22" x14ac:dyDescent="0.25">
@@ -2368,10 +2368,10 @@
         <v>45</v>
       </c>
       <c r="U49" s="3">
-        <v>84.377367688022289</v>
+        <v>90.54679533213644</v>
       </c>
       <c r="V49" s="3">
-        <v>231.58827777777779</v>
+        <v>253.77057347670251</v>
       </c>
     </row>
     <row r="50" spans="4:22" x14ac:dyDescent="0.25">
@@ -2410,10 +2410,10 @@
         <v>46</v>
       </c>
       <c r="U50" s="3">
-        <v>85.085731197771565</v>
+        <v>91.462118491921004</v>
       </c>
       <c r="V50" s="3">
-        <v>224.00155555555551</v>
+        <v>259.46132616487449</v>
       </c>
     </row>
     <row r="51" spans="4:22" x14ac:dyDescent="0.25">
@@ -2452,10 +2452,10 @@
         <v>47</v>
       </c>
       <c r="U51" s="3">
-        <v>82.008850974930368</v>
+        <v>94.578842010771965</v>
       </c>
       <c r="V51" s="3">
-        <v>270.76558333333332</v>
+        <v>248.9545519713262</v>
       </c>
     </row>
     <row r="52" spans="4:22" x14ac:dyDescent="0.25">
@@ -2494,10 +2494,10 @@
         <v>48</v>
       </c>
       <c r="U52" s="3">
-        <v>87.941357938718653</v>
+        <v>94.758393177737887</v>
       </c>
       <c r="V52" s="3">
-        <v>189.07472222222219</v>
+        <v>204.94483870967741</v>
       </c>
     </row>
     <row r="53" spans="4:22" x14ac:dyDescent="0.25">
@@ -2536,10 +2536,10 @@
         <v>49</v>
       </c>
       <c r="U53" s="3">
-        <v>84.578934540389966</v>
+        <v>99.753105924596042</v>
       </c>
       <c r="V53" s="3">
-        <v>236.17058333333341</v>
+        <v>199.9143727598566</v>
       </c>
     </row>
     <row r="54" spans="4:22" x14ac:dyDescent="0.25">
@@ -2578,10 +2578,10 @@
         <v>50</v>
       </c>
       <c r="U54" s="3">
-        <v>81.476497214484667</v>
+        <v>91.633806104129235</v>
       </c>
       <c r="V54" s="3">
-        <v>246.71838888888891</v>
+        <v>241.4994623655914</v>
       </c>
     </row>
     <row r="56" spans="4:22" x14ac:dyDescent="0.25">
@@ -2623,11 +2623,11 @@
       </c>
       <c r="U56" s="3">
         <f>AVERAGE(U5:U54)</f>
-        <v>83.550967827298066</v>
+        <v>92.994828007181354</v>
       </c>
       <c r="V56" s="3">
         <f>AVERAGE(V5:V54)</f>
-        <v>229.72429555555547</v>
+        <v>247.34961433691754</v>
       </c>
     </row>
     <row r="57" spans="4:22" x14ac:dyDescent="0.25">
@@ -2669,11 +2669,11 @@
       </c>
       <c r="U57" s="3">
         <f>_xlfn.STDEV.S(U5:U54)</f>
-        <v>2.1527115086902144</v>
+        <v>2.7562335707184586</v>
       </c>
       <c r="V57" s="3">
         <f>_xlfn.STDEV.S(V5:V54)</f>
-        <v>21.372741716027598</v>
+        <v>23.378577952467165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>